<commit_message>
add reference and update bab 2,3
</commit_message>
<xml_diff>
--- a/Hasil Uji.xlsx
+++ b/Hasil Uji.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Skenario 1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
   <si>
     <t>Precision</t>
   </si>
@@ -50,6 +50,12 @@
   </si>
   <si>
     <t>Tanpa PCA</t>
+  </si>
+  <si>
+    <t>Normalisasi</t>
+  </si>
+  <si>
+    <t>Tanpa Normalisasi</t>
   </si>
 </sst>
 </file>
@@ -1846,6 +1852,405 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="1" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>RECALL, PRECISION DAN F1 SCORE : OBSERVASI NORMALISASI</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Skenario 3'!$H$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Normalisasi</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Skenario 3'!$G$6:$G$8</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Recall</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Precision</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>F1 Score</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Skenario 3'!$H$6:$H$8</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Skenario 3'!$I$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Tanpa Normalisasi</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Skenario 3'!$G$6:$G$8</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Recall</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Precision</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>F1 Score</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Skenario 3'!$I$6:$I$8</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.67</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="-1337082544"/>
+        <c:axId val="-1337086896"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-1337082544"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1337086896"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-1337086896"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1337082544"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1938,6 +2343,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="207">
   <cs:axisTitle>
@@ -4115,6 +4560,509 @@
           <a:schemeClr val="lt1"/>
         </a:bgClr>
       </a:pattFill>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
     </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
@@ -4250,6 +5198,41 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>53340</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>163830</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>358140</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>163830</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -4515,8 +5498,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="H3:L6"/>
   <sheetViews>
-    <sheetView topLeftCell="B3" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3:L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4601,7 +5584,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D2:X13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
@@ -4996,12 +5979,63 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="G5:K8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q12" sqref="Q12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetData>
+    <row r="5" spans="7:11" x14ac:dyDescent="0.3">
+      <c r="H5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="7:11" x14ac:dyDescent="0.3">
+      <c r="G6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="I6" s="1">
+        <v>0.65</v>
+      </c>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+    </row>
+    <row r="7" spans="7:11" x14ac:dyDescent="0.3">
+      <c r="G7" t="s">
+        <v>0</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="I7" s="1">
+        <v>0.67</v>
+      </c>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+    </row>
+    <row r="8" spans="7:11" x14ac:dyDescent="0.3">
+      <c r="G8" t="s">
+        <v>1</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="I8" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update buku TA minus analisis bab 4
</commit_message>
<xml_diff>
--- a/Hasil Uji.xlsx
+++ b/Hasil Uji.xlsx
@@ -9,14 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Skenario 10-200" sheetId="4" r:id="rId1"/>
-    <sheet name="Skenario 45-65" sheetId="6" r:id="rId2"/>
-    <sheet name="Skenario Balanced Data" sheetId="7" r:id="rId3"/>
-    <sheet name="Skenario Normalisasi" sheetId="8" r:id="rId4"/>
-    <sheet name="Skenario 2" sheetId="2" r:id="rId5"/>
+    <sheet name="Grafik Eigenvalue" sheetId="9" r:id="rId2"/>
+    <sheet name="Skenario 45-65" sheetId="6" r:id="rId3"/>
+    <sheet name="Skenario Balanced Data" sheetId="7" r:id="rId4"/>
+    <sheet name="Skenario Normalisasi" sheetId="8" r:id="rId5"/>
+    <sheet name="Skenario 2" sheetId="2" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="682" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="21">
   <si>
     <t>Precision</t>
   </si>
@@ -83,6 +84,15 @@
   <si>
     <t>14-14 Normalisasi</t>
   </si>
+  <si>
+    <t>Eigenvalues</t>
+  </si>
+  <si>
+    <t>Nilai Eigen</t>
+  </si>
+  <si>
+    <t>Principal Component</t>
+  </si>
 </sst>
 </file>
 
@@ -112,7 +122,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -144,11 +154,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -174,12 +199,26 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -832,11 +871,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1373585776"/>
-        <c:axId val="-1373582512"/>
+        <c:axId val="1014199120"/>
+        <c:axId val="1014207280"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1373585776"/>
+        <c:axId val="1014199120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="200"/>
@@ -883,6 +922,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -949,13 +989,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1373582512"/>
+        <c:crossAx val="1014207280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="10"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1373582512"/>
+        <c:axId val="1014207280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1001,6 +1041,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1067,7 +1108,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1373585776"/>
+        <c:crossAx val="1014199120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1081,6 +1122,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1149,6 +1191,786 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>GRAFIK</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> NILAI EIGEN</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Grafik Eigenvalue'!$C$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Eigenvalues</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:alpha val="93000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Grafik Eigenvalue'!$D$8:$BK$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="60"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>60</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Grafik Eigenvalue'!$D$9:$BK$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="60"/>
+                <c:pt idx="0">
+                  <c:v>1292485.625</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>571133.3125</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>371341.0625</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>285117.875</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>248015.54689999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>188456.20310000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>166803.76560000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>148993.4063</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>134404.6563</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>127934.7344</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>117583.6094</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>108042.55469999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>101069.375</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>94869.78125</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>88263.390629999994</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>82613.71875</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>79780.609379999994</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>73653.0625</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>71713.375</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>65640.8125</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>62294.511720000002</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>60983.492189999997</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>59898.917970000002</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>56964.992189999997</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>53569.144529999998</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>52900.550779999998</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>52075.304689999997</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>47981.859380000002</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>46551.097659999999</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>45021.785159999999</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>44047.675779999998</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>43139.101560000003</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>41391.703130000002</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>39264.25</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>38659.769529999998</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>37485.414060000003</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>35557.121090000001</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>34089.953130000002</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>33440.558590000001</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>30962.51758</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>30558.550780000001</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>28655.875</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>27216.869139999999</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>26545.720700000002</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>26020.150389999999</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>24135.277340000001</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>22944.261719999999</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>22304.591799999998</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>21086.091799999998</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>20469.132809999999</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>20083.73242</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>17128.67383</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>15749.55176</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.19054579730000001</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.14288380740000001</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>1.7060473560000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>1.0675592350000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>8.3587337289999994E-3</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>7.9350788149999997E-3</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>5.308378953E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1014611072"/>
+        <c:axId val="1014611616"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1014611072"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" i="1"/>
+                  <a:t>Principal Component</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="t" anchorCtr="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1014611616"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="60"/>
+        <c:tickLblSkip val="1"/>
+        <c:tickMarkSkip val="1"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1014611616"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Nilai Eigen</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1014611072"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1289,10 +2111,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Skenario 45-65'!$G$166:$Z$166</c:f>
+              <c:f>'Skenario 45-65'!$G$166:$AA$166</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>45</c:v>
                 </c:pt>
@@ -1353,15 +2175,18 @@
                 <c:pt idx="19">
                   <c:v>64</c:v>
                 </c:pt>
+                <c:pt idx="20">
+                  <c:v>65</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Skenario 45-65'!$G$167:$Z$167</c:f>
+              <c:f>'Skenario 45-65'!$G$167:$AA$167</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>0.65835400000000011</c:v>
                 </c:pt>
@@ -1422,6 +2247,9 @@
                 <c:pt idx="19">
                   <c:v>0.84443800000000013</c:v>
                 </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.84451200000000004</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -1468,10 +2296,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Skenario 45-65'!$G$166:$Z$166</c:f>
+              <c:f>'Skenario 45-65'!$G$166:$AA$166</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>45</c:v>
                 </c:pt>
@@ -1532,15 +2360,18 @@
                 <c:pt idx="19">
                   <c:v>64</c:v>
                 </c:pt>
+                <c:pt idx="20">
+                  <c:v>65</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Skenario 45-65'!$G$168:$Z$168</c:f>
+              <c:f>'Skenario 45-65'!$G$168:$AA$168</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>0.87892600000000032</c:v>
                 </c:pt>
@@ -1601,6 +2432,9 @@
                 <c:pt idx="19">
                   <c:v>0.76076599999999994</c:v>
                 </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.76084999999999992</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -1648,10 +2482,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Skenario 45-65'!$G$166:$Z$166</c:f>
+              <c:f>'Skenario 45-65'!$G$166:$AA$166</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>45</c:v>
                 </c:pt>
@@ -1712,15 +2546,18 @@
                 <c:pt idx="19">
                   <c:v>64</c:v>
                 </c:pt>
+                <c:pt idx="20">
+                  <c:v>65</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Skenario 45-65'!$G$169:$Z$169</c:f>
+              <c:f>'Skenario 45-65'!$G$169:$AA$169</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>0.55498599999999998</c:v>
                 </c:pt>
@@ -1781,6 +2618,9 @@
                 <c:pt idx="19">
                   <c:v>0.99</c:v>
                 </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.99</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -1794,11 +2634,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1373574352"/>
-        <c:axId val="-1373580336"/>
+        <c:axId val="1014200208"/>
+        <c:axId val="1014200752"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1373574352"/>
+        <c:axId val="1014200208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="65"/>
@@ -1846,6 +2686,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1912,13 +2753,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1373580336"/>
+        <c:crossAx val="1014200752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1373580336"/>
+        <c:axId val="1014200752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1964,6 +2805,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2030,7 +2872,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1373574352"/>
+        <c:crossAx val="1014200208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2044,6 +2886,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2111,7 +2954,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2156,6 +2999,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2397,11 +3241,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-36"/>
-        <c:axId val="-1373572720"/>
-        <c:axId val="-1373577072"/>
+        <c:axId val="1014207824"/>
+        <c:axId val="1014210544"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1373572720"/>
+        <c:axId val="1014207824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2438,6 +3282,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2504,7 +3349,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1373577072"/>
+        <c:crossAx val="1014210544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2512,7 +3357,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1373577072"/>
+        <c:axId val="1014210544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2558,6 +3403,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2618,7 +3464,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1373572720"/>
+        <c:crossAx val="1014207824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2632,6 +3478,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2698,7 +3545,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -3049,11 +3896,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-36"/>
-        <c:axId val="-1373574896"/>
-        <c:axId val="-1373578160"/>
+        <c:axId val="1014210000"/>
+        <c:axId val="1014201840"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1373574896"/>
+        <c:axId val="1014210000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3157,7 +4004,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1373578160"/>
+        <c:crossAx val="1014201840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3165,7 +4012,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1373578160"/>
+        <c:axId val="1014201840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3272,7 +4119,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1373574896"/>
+        <c:crossAx val="1014210000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3474,6 +4321,46 @@
 </file>
 
 <file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -4034,6 +4921,509 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="241">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4553,7 +5943,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5056,7 +6446,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5598,6 +6988,41 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>77</xdr:col>
+      <xdr:colOff>182884</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>163833</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>77</xdr:col>
+      <xdr:colOff>480166</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>157771</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
       <xdr:row>171</xdr:row>
@@ -5631,7 +7056,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -5666,7 +7091,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -5968,7 +7393,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:Z169"/>
   <sheetViews>
-    <sheetView topLeftCell="D35" workbookViewId="0">
+    <sheetView topLeftCell="G173" workbookViewId="0">
       <selection activeCell="E57" sqref="E57"/>
     </sheetView>
   </sheetViews>
@@ -9602,10 +11027,10 @@
       </c>
     </row>
     <row r="55" spans="3:26" x14ac:dyDescent="0.3">
-      <c r="E55" s="11" t="s">
+      <c r="E55" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="F55" s="11"/>
+      <c r="F55" s="12"/>
       <c r="G55" s="7"/>
       <c r="H55" s="7"/>
     </row>
@@ -17070,6 +18495,1056 @@
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="E55:F55"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C8:CY24"/>
+  <sheetViews>
+    <sheetView zoomScale="92" zoomScaleNormal="92" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17:M24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="8.88671875" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="8" spans="3:103" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="F8">
+        <v>3</v>
+      </c>
+      <c r="G8">
+        <v>4</v>
+      </c>
+      <c r="H8">
+        <v>5</v>
+      </c>
+      <c r="I8">
+        <v>6</v>
+      </c>
+      <c r="J8">
+        <v>7</v>
+      </c>
+      <c r="K8">
+        <v>8</v>
+      </c>
+      <c r="L8">
+        <v>9</v>
+      </c>
+      <c r="M8">
+        <v>10</v>
+      </c>
+      <c r="N8">
+        <v>11</v>
+      </c>
+      <c r="O8">
+        <v>12</v>
+      </c>
+      <c r="P8">
+        <v>13</v>
+      </c>
+      <c r="Q8">
+        <v>14</v>
+      </c>
+      <c r="R8">
+        <v>15</v>
+      </c>
+      <c r="S8">
+        <v>16</v>
+      </c>
+      <c r="T8">
+        <v>17</v>
+      </c>
+      <c r="U8">
+        <v>18</v>
+      </c>
+      <c r="V8">
+        <v>19</v>
+      </c>
+      <c r="W8">
+        <v>20</v>
+      </c>
+      <c r="X8">
+        <v>21</v>
+      </c>
+      <c r="Y8">
+        <v>22</v>
+      </c>
+      <c r="Z8">
+        <v>23</v>
+      </c>
+      <c r="AA8">
+        <v>24</v>
+      </c>
+      <c r="AB8">
+        <v>25</v>
+      </c>
+      <c r="AC8">
+        <v>26</v>
+      </c>
+      <c r="AD8">
+        <v>27</v>
+      </c>
+      <c r="AE8">
+        <v>28</v>
+      </c>
+      <c r="AF8">
+        <v>29</v>
+      </c>
+      <c r="AG8">
+        <v>30</v>
+      </c>
+      <c r="AH8">
+        <v>31</v>
+      </c>
+      <c r="AI8">
+        <v>32</v>
+      </c>
+      <c r="AJ8">
+        <v>33</v>
+      </c>
+      <c r="AK8">
+        <v>34</v>
+      </c>
+      <c r="AL8">
+        <v>35</v>
+      </c>
+      <c r="AM8">
+        <v>36</v>
+      </c>
+      <c r="AN8">
+        <v>37</v>
+      </c>
+      <c r="AO8">
+        <v>38</v>
+      </c>
+      <c r="AP8">
+        <v>39</v>
+      </c>
+      <c r="AQ8">
+        <v>40</v>
+      </c>
+      <c r="AR8">
+        <v>41</v>
+      </c>
+      <c r="AS8">
+        <v>42</v>
+      </c>
+      <c r="AT8">
+        <v>43</v>
+      </c>
+      <c r="AU8">
+        <v>44</v>
+      </c>
+      <c r="AV8">
+        <v>45</v>
+      </c>
+      <c r="AW8">
+        <v>46</v>
+      </c>
+      <c r="AX8">
+        <v>47</v>
+      </c>
+      <c r="AY8">
+        <v>48</v>
+      </c>
+      <c r="AZ8">
+        <v>49</v>
+      </c>
+      <c r="BA8">
+        <v>50</v>
+      </c>
+      <c r="BB8">
+        <v>51</v>
+      </c>
+      <c r="BC8">
+        <v>52</v>
+      </c>
+      <c r="BD8">
+        <v>53</v>
+      </c>
+      <c r="BE8">
+        <v>54</v>
+      </c>
+      <c r="BF8">
+        <v>55</v>
+      </c>
+      <c r="BG8">
+        <v>56</v>
+      </c>
+      <c r="BH8">
+        <v>57</v>
+      </c>
+      <c r="BI8">
+        <v>58</v>
+      </c>
+      <c r="BJ8">
+        <v>59</v>
+      </c>
+      <c r="BK8">
+        <v>60</v>
+      </c>
+      <c r="BL8">
+        <v>61</v>
+      </c>
+      <c r="BM8">
+        <v>62</v>
+      </c>
+      <c r="BN8">
+        <v>63</v>
+      </c>
+      <c r="BO8">
+        <v>64</v>
+      </c>
+      <c r="BP8">
+        <v>65</v>
+      </c>
+      <c r="BQ8">
+        <v>66</v>
+      </c>
+      <c r="BR8">
+        <v>67</v>
+      </c>
+      <c r="BS8">
+        <v>68</v>
+      </c>
+      <c r="BT8">
+        <v>69</v>
+      </c>
+      <c r="BU8">
+        <v>70</v>
+      </c>
+      <c r="BV8">
+        <v>71</v>
+      </c>
+      <c r="BW8">
+        <v>72</v>
+      </c>
+      <c r="BX8">
+        <v>73</v>
+      </c>
+      <c r="BY8">
+        <v>74</v>
+      </c>
+      <c r="BZ8">
+        <v>75</v>
+      </c>
+      <c r="CA8">
+        <v>76</v>
+      </c>
+      <c r="CB8">
+        <v>77</v>
+      </c>
+      <c r="CC8">
+        <v>78</v>
+      </c>
+      <c r="CD8">
+        <v>79</v>
+      </c>
+      <c r="CE8">
+        <v>80</v>
+      </c>
+      <c r="CF8">
+        <v>81</v>
+      </c>
+      <c r="CG8">
+        <v>82</v>
+      </c>
+      <c r="CH8">
+        <v>83</v>
+      </c>
+      <c r="CI8">
+        <v>84</v>
+      </c>
+      <c r="CJ8">
+        <v>85</v>
+      </c>
+      <c r="CK8">
+        <v>86</v>
+      </c>
+      <c r="CL8">
+        <v>87</v>
+      </c>
+      <c r="CM8">
+        <v>88</v>
+      </c>
+      <c r="CN8">
+        <v>89</v>
+      </c>
+      <c r="CO8">
+        <v>90</v>
+      </c>
+      <c r="CP8">
+        <v>91</v>
+      </c>
+      <c r="CQ8">
+        <v>92</v>
+      </c>
+      <c r="CR8">
+        <v>93</v>
+      </c>
+      <c r="CS8">
+        <v>94</v>
+      </c>
+      <c r="CT8">
+        <v>95</v>
+      </c>
+      <c r="CU8">
+        <v>96</v>
+      </c>
+      <c r="CV8">
+        <v>97</v>
+      </c>
+      <c r="CW8">
+        <v>98</v>
+      </c>
+      <c r="CX8">
+        <v>99</v>
+      </c>
+      <c r="CY8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="3:103" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="3">
+        <v>1292485.625</v>
+      </c>
+      <c r="E9" s="3">
+        <v>571133.3125</v>
+      </c>
+      <c r="F9" s="3">
+        <v>371341.0625</v>
+      </c>
+      <c r="G9" s="3">
+        <v>285117.875</v>
+      </c>
+      <c r="H9" s="3">
+        <v>248015.54689999999</v>
+      </c>
+      <c r="I9" s="3">
+        <v>188456.20310000001</v>
+      </c>
+      <c r="J9" s="3">
+        <v>166803.76560000001</v>
+      </c>
+      <c r="K9" s="3">
+        <v>148993.4063</v>
+      </c>
+      <c r="L9" s="3">
+        <v>134404.6563</v>
+      </c>
+      <c r="M9" s="3">
+        <v>127934.7344</v>
+      </c>
+      <c r="N9" s="3">
+        <v>117583.6094</v>
+      </c>
+      <c r="O9" s="3">
+        <v>108042.55469999999</v>
+      </c>
+      <c r="P9" s="3">
+        <v>101069.375</v>
+      </c>
+      <c r="Q9" s="3">
+        <v>94869.78125</v>
+      </c>
+      <c r="R9" s="3">
+        <v>88263.390629999994</v>
+      </c>
+      <c r="S9" s="3">
+        <v>82613.71875</v>
+      </c>
+      <c r="T9" s="3">
+        <v>79780.609379999994</v>
+      </c>
+      <c r="U9" s="3">
+        <v>73653.0625</v>
+      </c>
+      <c r="V9" s="3">
+        <v>71713.375</v>
+      </c>
+      <c r="W9" s="3">
+        <v>65640.8125</v>
+      </c>
+      <c r="X9" s="3">
+        <v>62294.511720000002</v>
+      </c>
+      <c r="Y9" s="3">
+        <v>60983.492189999997</v>
+      </c>
+      <c r="Z9" s="3">
+        <v>59898.917970000002</v>
+      </c>
+      <c r="AA9" s="3">
+        <v>56964.992189999997</v>
+      </c>
+      <c r="AB9" s="3">
+        <v>53569.144529999998</v>
+      </c>
+      <c r="AC9" s="3">
+        <v>52900.550779999998</v>
+      </c>
+      <c r="AD9" s="3">
+        <v>52075.304689999997</v>
+      </c>
+      <c r="AE9" s="3">
+        <v>47981.859380000002</v>
+      </c>
+      <c r="AF9" s="3">
+        <v>46551.097659999999</v>
+      </c>
+      <c r="AG9" s="3">
+        <v>45021.785159999999</v>
+      </c>
+      <c r="AH9" s="3">
+        <v>44047.675779999998</v>
+      </c>
+      <c r="AI9" s="3">
+        <v>43139.101560000003</v>
+      </c>
+      <c r="AJ9" s="3">
+        <v>41391.703130000002</v>
+      </c>
+      <c r="AK9" s="3">
+        <v>39264.25</v>
+      </c>
+      <c r="AL9" s="3">
+        <v>38659.769529999998</v>
+      </c>
+      <c r="AM9" s="3">
+        <v>37485.414060000003</v>
+      </c>
+      <c r="AN9" s="3">
+        <v>35557.121090000001</v>
+      </c>
+      <c r="AO9" s="3">
+        <v>34089.953130000002</v>
+      </c>
+      <c r="AP9" s="3">
+        <v>33440.558590000001</v>
+      </c>
+      <c r="AQ9" s="3">
+        <v>30962.51758</v>
+      </c>
+      <c r="AR9" s="3">
+        <v>30558.550780000001</v>
+      </c>
+      <c r="AS9" s="3">
+        <v>28655.875</v>
+      </c>
+      <c r="AT9" s="3">
+        <v>27216.869139999999</v>
+      </c>
+      <c r="AU9" s="3">
+        <v>26545.720700000002</v>
+      </c>
+      <c r="AV9" s="3">
+        <v>26020.150389999999</v>
+      </c>
+      <c r="AW9" s="3">
+        <v>24135.277340000001</v>
+      </c>
+      <c r="AX9" s="3">
+        <v>22944.261719999999</v>
+      </c>
+      <c r="AY9" s="3">
+        <v>22304.591799999998</v>
+      </c>
+      <c r="AZ9" s="3">
+        <v>21086.091799999998</v>
+      </c>
+      <c r="BA9" s="3">
+        <v>20469.132809999999</v>
+      </c>
+      <c r="BB9" s="3">
+        <v>20083.73242</v>
+      </c>
+      <c r="BC9" s="3">
+        <v>17128.67383</v>
+      </c>
+      <c r="BD9" s="3">
+        <v>15749.55176</v>
+      </c>
+      <c r="BE9" s="3">
+        <v>0.19054579730000001</v>
+      </c>
+      <c r="BF9" s="3">
+        <v>0.14288380740000001</v>
+      </c>
+      <c r="BG9" s="3">
+        <v>1.7060473560000001E-2</v>
+      </c>
+      <c r="BH9" s="3">
+        <v>1.0675592350000001E-2</v>
+      </c>
+      <c r="BI9" s="3">
+        <v>8.3587337289999994E-3</v>
+      </c>
+      <c r="BJ9" s="3">
+        <v>7.9350788149999997E-3</v>
+      </c>
+      <c r="BK9" s="3">
+        <v>5.308378953E-3</v>
+      </c>
+      <c r="BL9" s="3">
+        <v>4.9686497080000001E-3</v>
+      </c>
+      <c r="BM9" s="3">
+        <v>4.5846127900000004E-3</v>
+      </c>
+      <c r="BN9" s="3">
+        <v>4.4699446300000001E-3</v>
+      </c>
+      <c r="BO9" s="3">
+        <v>4.2620939199999996E-3</v>
+      </c>
+      <c r="BP9" s="3">
+        <v>4.2328904380000004E-3</v>
+      </c>
+      <c r="BQ9" s="3">
+        <v>3.8021081130000002E-3</v>
+      </c>
+      <c r="BR9" s="3">
+        <v>3.7033562549999999E-3</v>
+      </c>
+      <c r="BS9" s="3">
+        <v>3.701995127E-3</v>
+      </c>
+      <c r="BT9" s="3">
+        <v>3.6444049330000001E-3</v>
+      </c>
+      <c r="BU9" s="3">
+        <v>3.6387215370000002E-3</v>
+      </c>
+      <c r="BV9" s="3">
+        <v>3.1510721890000001E-3</v>
+      </c>
+      <c r="BW9" s="3">
+        <v>3.0506388280000002E-3</v>
+      </c>
+      <c r="BX9" s="3">
+        <v>2.8737119860000001E-3</v>
+      </c>
+      <c r="BY9" s="3">
+        <v>2.6936279610000002E-3</v>
+      </c>
+      <c r="BZ9" s="3">
+        <v>2.5327675979999998E-3</v>
+      </c>
+      <c r="CA9" s="3">
+        <v>2.2992789750000001E-3</v>
+      </c>
+      <c r="CB9" s="3">
+        <v>2.1428316829999999E-3</v>
+      </c>
+      <c r="CC9" s="3">
+        <v>1.8126112409999999E-3</v>
+      </c>
+      <c r="CD9" s="3">
+        <v>1.209605951E-3</v>
+      </c>
+      <c r="CE9" s="3">
+        <v>1.0924842210000001E-3</v>
+      </c>
+      <c r="CF9" s="3">
+        <v>6.1016681140000002E-4</v>
+      </c>
+      <c r="CG9" s="3">
+        <v>5.0084886610000001E-4</v>
+      </c>
+      <c r="CH9" s="3">
+        <v>4.6554519210000001E-4</v>
+      </c>
+      <c r="CI9" s="3">
+        <v>4.5364556719999999E-4</v>
+      </c>
+      <c r="CJ9" s="3">
+        <v>4.4461604560000001E-4</v>
+      </c>
+      <c r="CK9" s="3">
+        <v>4.323594912E-4</v>
+      </c>
+      <c r="CL9" s="3">
+        <v>3.9864284919999997E-4</v>
+      </c>
+      <c r="CM9" s="3">
+        <v>3.8191216299999998E-4</v>
+      </c>
+      <c r="CN9" s="3">
+        <v>3.785080626E-4</v>
+      </c>
+      <c r="CO9" s="3">
+        <v>3.6696909229999998E-4</v>
+      </c>
+      <c r="CP9" s="3">
+        <v>3.6074535460000001E-4</v>
+      </c>
+      <c r="CQ9" s="3">
+        <v>3.5671010849999999E-4</v>
+      </c>
+      <c r="CR9" s="3">
+        <v>3.459500149E-4</v>
+      </c>
+      <c r="CS9" s="3">
+        <v>3.4583173690000001E-4</v>
+      </c>
+      <c r="CT9" s="3">
+        <v>3.4330954080000003E-4</v>
+      </c>
+      <c r="CU9" s="3">
+        <v>3.428307537E-4</v>
+      </c>
+      <c r="CV9" s="3">
+        <v>3.4148950360000002E-4</v>
+      </c>
+      <c r="CW9" s="3">
+        <v>3.412476217E-4</v>
+      </c>
+      <c r="CX9" s="3">
+        <v>3.3419794639999998E-4</v>
+      </c>
+      <c r="CY9" s="3">
+        <v>3.315269132E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="3:103" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D10" s="3">
+        <v>117583.6094</v>
+      </c>
+      <c r="E10" s="3">
+        <v>108042.55469999999</v>
+      </c>
+      <c r="F10" s="3">
+        <v>101069.375</v>
+      </c>
+      <c r="G10" s="3">
+        <v>94869.78125</v>
+      </c>
+      <c r="H10" s="3">
+        <v>88263.390629999994</v>
+      </c>
+      <c r="I10" s="3">
+        <v>82613.71875</v>
+      </c>
+      <c r="J10" s="3">
+        <v>79780.609379999994</v>
+      </c>
+      <c r="K10" s="3">
+        <v>73653.0625</v>
+      </c>
+      <c r="L10" s="3">
+        <v>71713.375</v>
+      </c>
+      <c r="M10" s="3">
+        <v>65640.8125</v>
+      </c>
+    </row>
+    <row r="11" spans="3:103" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D11" s="3">
+        <v>62294.511720000002</v>
+      </c>
+      <c r="E11" s="3">
+        <v>60983.492189999997</v>
+      </c>
+      <c r="F11" s="3">
+        <v>59898.917970000002</v>
+      </c>
+      <c r="G11" s="3">
+        <v>56964.992189999997</v>
+      </c>
+      <c r="H11" s="3">
+        <v>53569.144529999998</v>
+      </c>
+      <c r="I11" s="3">
+        <v>52900.550779999998</v>
+      </c>
+      <c r="J11" s="3">
+        <v>52075.304689999997</v>
+      </c>
+      <c r="K11" s="3">
+        <v>47981.859380000002</v>
+      </c>
+      <c r="L11" s="3">
+        <v>46551.097659999999</v>
+      </c>
+      <c r="M11" s="3">
+        <v>45021.785159999999</v>
+      </c>
+    </row>
+    <row r="12" spans="3:103" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D12" s="3">
+        <v>44047.675779999998</v>
+      </c>
+      <c r="E12" s="3">
+        <v>43139.101560000003</v>
+      </c>
+      <c r="F12" s="3">
+        <v>41391.703130000002</v>
+      </c>
+      <c r="G12" s="3">
+        <v>39264.25</v>
+      </c>
+      <c r="H12" s="3">
+        <v>38659.769529999998</v>
+      </c>
+      <c r="I12" s="3">
+        <v>37485.414060000003</v>
+      </c>
+      <c r="J12" s="3">
+        <v>35557.121090000001</v>
+      </c>
+      <c r="K12" s="3">
+        <v>34089.953130000002</v>
+      </c>
+      <c r="L12" s="3">
+        <v>33440.558590000001</v>
+      </c>
+      <c r="M12" s="3">
+        <v>30962.51758</v>
+      </c>
+      <c r="N12" s="3"/>
+    </row>
+    <row r="13" spans="3:103" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D13" s="3">
+        <v>30558.550780000001</v>
+      </c>
+      <c r="E13" s="3">
+        <v>28655.875</v>
+      </c>
+      <c r="F13" s="3">
+        <v>27216.869139999999</v>
+      </c>
+      <c r="G13" s="3">
+        <v>26545.720700000002</v>
+      </c>
+      <c r="H13" s="3">
+        <v>26020.150389999999</v>
+      </c>
+      <c r="I13" s="3">
+        <v>24135.277340000001</v>
+      </c>
+      <c r="J13" s="3">
+        <v>22944.261719999999</v>
+      </c>
+      <c r="K13" s="3">
+        <v>22304.591799999998</v>
+      </c>
+      <c r="L13" s="3">
+        <v>21086.091799999998</v>
+      </c>
+      <c r="M13" s="3">
+        <v>20469.132809999999</v>
+      </c>
+    </row>
+    <row r="14" spans="3:103" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D14" s="3">
+        <v>20083.73242</v>
+      </c>
+      <c r="E14" s="3">
+        <v>17128.67383</v>
+      </c>
+      <c r="F14" s="3">
+        <v>15749.55176</v>
+      </c>
+      <c r="G14" s="3">
+        <v>0.19054579730000001</v>
+      </c>
+      <c r="H14" s="3">
+        <v>0.14288380740000001</v>
+      </c>
+      <c r="I14" s="3">
+        <v>1.7060473560000001E-2</v>
+      </c>
+      <c r="J14" s="3">
+        <v>1.0675592350000001E-2</v>
+      </c>
+      <c r="K14" s="3">
+        <v>8.3587337289999994E-3</v>
+      </c>
+      <c r="L14" s="3">
+        <v>7.9350788149999997E-3</v>
+      </c>
+      <c r="M14" s="3">
+        <v>5.308378953E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C17" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="13"/>
+      <c r="L17" s="13"/>
+      <c r="M17" s="13"/>
+    </row>
+    <row r="18" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C18" s="14"/>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
+      <c r="F18">
+        <v>3</v>
+      </c>
+      <c r="G18">
+        <v>4</v>
+      </c>
+      <c r="H18">
+        <v>5</v>
+      </c>
+      <c r="I18">
+        <v>6</v>
+      </c>
+      <c r="J18">
+        <v>7</v>
+      </c>
+      <c r="K18">
+        <v>8</v>
+      </c>
+      <c r="L18">
+        <v>9</v>
+      </c>
+      <c r="M18">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D19" s="3">
+        <v>1292485.625</v>
+      </c>
+      <c r="E19" s="3">
+        <v>571133.3125</v>
+      </c>
+      <c r="F19" s="3">
+        <v>371341.0625</v>
+      </c>
+      <c r="G19" s="3">
+        <v>285117.875</v>
+      </c>
+      <c r="H19" s="3">
+        <v>248015.54689999999</v>
+      </c>
+      <c r="I19" s="3">
+        <v>188456.20310000001</v>
+      </c>
+      <c r="J19" s="3">
+        <v>166803.76560000001</v>
+      </c>
+      <c r="K19" s="3">
+        <v>148993.4063</v>
+      </c>
+      <c r="L19" s="3">
+        <v>134404.6563</v>
+      </c>
+      <c r="M19" s="3">
+        <v>127934.7344</v>
+      </c>
+    </row>
+    <row r="20" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C20">
+        <v>11</v>
+      </c>
+      <c r="D20" s="3">
+        <v>117583.6094</v>
+      </c>
+      <c r="E20" s="3">
+        <v>108042.55469999999</v>
+      </c>
+      <c r="F20" s="3">
+        <v>101069.375</v>
+      </c>
+      <c r="G20" s="3">
+        <v>94869.78125</v>
+      </c>
+      <c r="H20" s="3">
+        <v>88263.390629999994</v>
+      </c>
+      <c r="I20" s="3">
+        <v>82613.71875</v>
+      </c>
+      <c r="J20" s="3">
+        <v>79780.609379999994</v>
+      </c>
+      <c r="K20" s="3">
+        <v>73653.0625</v>
+      </c>
+      <c r="L20" s="3">
+        <v>71713.375</v>
+      </c>
+      <c r="M20" s="3">
+        <v>65640.8125</v>
+      </c>
+    </row>
+    <row r="21" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C21">
+        <v>21</v>
+      </c>
+      <c r="D21" s="3">
+        <v>62294.511720000002</v>
+      </c>
+      <c r="E21" s="3">
+        <v>60983.492189999997</v>
+      </c>
+      <c r="F21" s="3">
+        <v>59898.917970000002</v>
+      </c>
+      <c r="G21" s="3">
+        <v>56964.992189999997</v>
+      </c>
+      <c r="H21" s="3">
+        <v>53569.144529999998</v>
+      </c>
+      <c r="I21" s="3">
+        <v>52900.550779999998</v>
+      </c>
+      <c r="J21" s="3">
+        <v>52075.304689999997</v>
+      </c>
+      <c r="K21" s="3">
+        <v>47981.859380000002</v>
+      </c>
+      <c r="L21" s="3">
+        <v>46551.097659999999</v>
+      </c>
+      <c r="M21" s="3">
+        <v>45021.785159999999</v>
+      </c>
+    </row>
+    <row r="22" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C22">
+        <v>31</v>
+      </c>
+      <c r="D22" s="3">
+        <v>44047.675779999998</v>
+      </c>
+      <c r="E22" s="3">
+        <v>43139.101560000003</v>
+      </c>
+      <c r="F22" s="3">
+        <v>41391.703130000002</v>
+      </c>
+      <c r="G22" s="3">
+        <v>39264.25</v>
+      </c>
+      <c r="H22" s="3">
+        <v>38659.769529999998</v>
+      </c>
+      <c r="I22" s="3">
+        <v>37485.414060000003</v>
+      </c>
+      <c r="J22" s="3">
+        <v>35557.121090000001</v>
+      </c>
+      <c r="K22" s="3">
+        <v>34089.953130000002</v>
+      </c>
+      <c r="L22" s="3">
+        <v>33440.558590000001</v>
+      </c>
+      <c r="M22" s="3">
+        <v>30962.51758</v>
+      </c>
+    </row>
+    <row r="23" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C23">
+        <v>41</v>
+      </c>
+      <c r="D23" s="3">
+        <v>30558.550780000001</v>
+      </c>
+      <c r="E23" s="3">
+        <v>28655.875</v>
+      </c>
+      <c r="F23" s="3">
+        <v>27216.869139999999</v>
+      </c>
+      <c r="G23" s="3">
+        <v>26545.720700000002</v>
+      </c>
+      <c r="H23" s="3">
+        <v>26020.150389999999</v>
+      </c>
+      <c r="I23" s="3">
+        <v>24135.277340000001</v>
+      </c>
+      <c r="J23" s="3">
+        <v>22944.261719999999</v>
+      </c>
+      <c r="K23" s="3">
+        <v>22304.591799999998</v>
+      </c>
+      <c r="L23" s="3">
+        <v>21086.091799999998</v>
+      </c>
+      <c r="M23" s="3">
+        <v>20469.132809999999</v>
+      </c>
+    </row>
+    <row r="24" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C24">
+        <v>51</v>
+      </c>
+      <c r="D24" s="3">
+        <v>20083.73242</v>
+      </c>
+      <c r="E24" s="3">
+        <v>17128.67383</v>
+      </c>
+      <c r="F24" s="3">
+        <v>15749.55176</v>
+      </c>
+      <c r="G24" s="3">
+        <v>0.19054579730000001</v>
+      </c>
+      <c r="H24" s="3">
+        <v>0.14288380740000001</v>
+      </c>
+      <c r="I24" s="3">
+        <v>1.7060473560000001E-2</v>
+      </c>
+      <c r="J24" s="3">
+        <v>1.0675592350000001E-2</v>
+      </c>
+      <c r="K24" s="3">
+        <v>8.3587337289999994E-3</v>
+      </c>
+      <c r="L24" s="3">
+        <v>7.9350788149999997E-3</v>
+      </c>
+      <c r="M24" s="3">
+        <v>5.308378953E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="D17:M17"/>
+    <mergeCell ref="C17:C18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -17077,11 +19552,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:AA169"/>
   <sheetViews>
-    <sheetView topLeftCell="A172" workbookViewId="0">
+    <sheetView topLeftCell="E163" workbookViewId="0">
       <selection activeCell="O113" sqref="O113:O162"/>
     </sheetView>
   </sheetViews>
@@ -28645,12 +31120,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:Z169"/>
   <sheetViews>
     <sheetView topLeftCell="A163" workbookViewId="0">
-      <selection activeCell="B182" sqref="B182"/>
+      <selection activeCell="F166" sqref="F166:I169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -34215,12 +36690,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:Z169"/>
+  <dimension ref="C3:Z171"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D163" workbookViewId="0">
-      <selection activeCell="L181" sqref="L181"/>
+      <selection activeCell="L171" sqref="L171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -34253,13 +36728,13 @@
       <c r="H4" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="I4" s="12" t="s">
+      <c r="I4" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="J4" s="12" t="s">
+      <c r="J4" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="K4" s="12" t="s">
+      <c r="K4" s="11" t="s">
         <v>17</v>
       </c>
     </row>
@@ -36416,13 +38891,13 @@
       <c r="H58" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="I58" s="12" t="s">
+      <c r="I58" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="J58" s="12" t="s">
+      <c r="J58" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="K58" s="12" t="s">
+      <c r="K58" s="11" t="s">
         <v>17</v>
       </c>
     </row>
@@ -38536,13 +41011,13 @@
       <c r="H112" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="I112" s="12" t="s">
+      <c r="I112" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="J112" s="12" t="s">
+      <c r="J112" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="K112" s="12" t="s">
+      <c r="K112" s="11" t="s">
         <v>17</v>
       </c>
     </row>
@@ -40641,45 +43116,46 @@
       <c r="Z164" s="5"/>
     </row>
     <row r="166" spans="3:26" x14ac:dyDescent="0.3">
-      <c r="G166" s="8" t="s">
+      <c r="F166" s="15"/>
+      <c r="G166" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="H166" s="12" t="s">
+      <c r="H166" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="I166" s="8" t="s">
+      <c r="I166" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="J166" s="12" t="s">
+      <c r="J166" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="K166" s="8" t="s">
+      <c r="K166" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="L166" s="12" t="s">
+      <c r="L166" s="17" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="167" spans="3:26" x14ac:dyDescent="0.3">
-      <c r="F167" t="s">
-        <v>1</v>
-      </c>
-      <c r="G167" s="5">
+      <c r="F167" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="G167" s="18">
         <v>0.84758600000000006</v>
       </c>
-      <c r="H167" s="5">
+      <c r="H167" s="18">
         <v>0.82895399999999997</v>
       </c>
-      <c r="I167" s="5">
+      <c r="I167" s="18">
         <v>0.38746999999999993</v>
       </c>
-      <c r="J167" s="5">
+      <c r="J167" s="18">
         <v>0.36881399999999998</v>
       </c>
-      <c r="K167" s="5">
+      <c r="K167" s="18">
         <v>0.28156999999999999</v>
       </c>
-      <c r="L167" s="5">
+      <c r="L167" s="18">
         <v>0.19341599999999995</v>
       </c>
       <c r="M167" s="5"/>
@@ -40697,25 +43173,25 @@
       <c r="Z167" s="5"/>
     </row>
     <row r="168" spans="3:26" x14ac:dyDescent="0.3">
-      <c r="F168" t="s">
+      <c r="F168" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="G168" s="5">
+      <c r="G168" s="18">
         <v>0.76448399999999983</v>
       </c>
-      <c r="H168" s="5">
+      <c r="H168" s="18">
         <v>0.74027400000000032</v>
       </c>
-      <c r="I168" s="5">
+      <c r="I168" s="18">
         <v>0.49225000000000002</v>
       </c>
-      <c r="J168" s="5">
+      <c r="J168" s="18">
         <v>0.41716600000000009</v>
       </c>
-      <c r="K168" s="5">
+      <c r="K168" s="18">
         <v>0.23591400000000001</v>
       </c>
-      <c r="L168" s="5">
+      <c r="L168" s="18">
         <v>0.16008399999999998</v>
       </c>
       <c r="M168" s="5"/>
@@ -40733,25 +43209,25 @@
       <c r="Z168" s="5"/>
     </row>
     <row r="169" spans="3:26" x14ac:dyDescent="0.3">
-      <c r="F169" t="s">
+      <c r="F169" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="G169" s="5">
+      <c r="G169" s="18">
         <v>0.99</v>
       </c>
-      <c r="H169" s="5">
+      <c r="H169" s="18">
         <v>0.98499999999999999</v>
       </c>
-      <c r="I169" s="5">
+      <c r="I169" s="18">
         <v>0.38241799999999981</v>
       </c>
-      <c r="J169" s="5">
+      <c r="J169" s="18">
         <v>0.40345000000000009</v>
       </c>
-      <c r="K169" s="5">
+      <c r="K169" s="18">
         <v>0.463752</v>
       </c>
-      <c r="L169" s="5">
+      <c r="L169" s="18">
         <v>0.316334</v>
       </c>
       <c r="M169" s="5"/>
@@ -40768,6 +43244,9 @@
       <c r="Y169" s="5"/>
       <c r="Z169" s="5"/>
     </row>
+    <row r="171" spans="3:26" x14ac:dyDescent="0.3">
+      <c r="I171" s="15"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -40775,7 +43254,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="E3:X13"/>
   <sheetViews>

</xml_diff>

<commit_message>
update buku TA bab 4 kurang skenari 3 dan kesimpulan di bab 5
</commit_message>
<xml_diff>
--- a/Hasil Uji.xlsx
+++ b/Hasil Uji.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384"/>
   </bookViews>
   <sheets>
     <sheet name="Skenario 10-200" sheetId="4" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="21">
   <si>
     <t>Precision</t>
   </si>
@@ -114,12 +114,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="4">
@@ -173,7 +179,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -202,6 +208,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -211,14 +225,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -273,7 +281,30 @@
               <a:rPr lang="en-US" sz="1800" b="1" i="0" baseline="0">
                 <a:effectLst/>
               </a:rPr>
-              <a:t>RECALL, PRECISION DAN F1 SCORE : OBSERVASI Jumlah komponen 10-200</a:t>
+              <a:t>RECALL, PRECISION DAN F1 SCORE : </a:t>
+            </a:r>
+            <a:br>
+              <a:rPr lang="en-US" sz="1800" b="1" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+            </a:br>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="1" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>OBSERVASI </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="1" i="1" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>PRINCIPAL ComponenT</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="1" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t> 10-200</a:t>
             </a:r>
             <a:endParaRPr lang="en-US">
               <a:effectLst/>
@@ -285,8 +316,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.11726726726726729"/>
-          <c:y val="3.0054348767195805E-2"/>
+          <c:x val="0.16981981981981986"/>
+          <c:y val="3.6337729225882583E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -871,11 +902,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1014199120"/>
-        <c:axId val="1014207280"/>
+        <c:axId val="160929552"/>
+        <c:axId val="160931728"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1014199120"/>
+        <c:axId val="160929552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="200"/>
@@ -916,8 +947,8 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Jumlah komponen</a:t>
+                  <a:rPr lang="en-US" i="1"/>
+                  <a:t>PRINCIPAL COMPONENT</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -989,13 +1020,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1014207280"/>
+        <c:crossAx val="160931728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="10"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1014207280"/>
+        <c:axId val="160931728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1108,7 +1139,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1014199120"/>
+        <c:crossAx val="160929552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1235,7 +1266,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1701,11 +1731,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1014611072"/>
-        <c:axId val="1014611616"/>
+        <c:axId val="160932272"/>
+        <c:axId val="160932816"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1014611072"/>
+        <c:axId val="160932272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1737,7 +1767,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1785,7 +1814,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="t" anchorCtr="0"/>
+          <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="t" anchorCtr="0"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -1804,7 +1833,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1014611616"/>
+        <c:crossAx val="160932816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1814,7 +1843,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1014611616"/>
+        <c:axId val="160932816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1860,7 +1889,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1921,7 +1949,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1014611072"/>
+        <c:crossAx val="160932272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1990,7 +2018,7 @@
           <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
-            <a:pPr>
+            <a:pPr algn="ctr">
               <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
@@ -2018,7 +2046,19 @@
               <a:rPr lang="en-US" sz="1800" b="1" i="0" baseline="0">
                 <a:effectLst/>
               </a:rPr>
-              <a:t>OBSERVASI Jumlah komponen 45-65</a:t>
+              <a:t>OBSERVASI </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="1" i="1" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>PRINCIPAL COMPONENT</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="1" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t> 45-65</a:t>
             </a:r>
             <a:endParaRPr lang="en-US">
               <a:effectLst/>
@@ -2030,8 +2070,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.11726726726726729"/>
-          <c:y val="3.0054348767195805E-2"/>
+          <c:x val="0.18231654983000542"/>
+          <c:y val="3.292056248772858E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -2046,7 +2086,7 @@
         <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
         <a:lstStyle/>
         <a:p>
-          <a:pPr>
+          <a:pPr algn="ctr">
             <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
@@ -2634,11 +2674,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1014200208"/>
-        <c:axId val="1014200752"/>
+        <c:axId val="160936624"/>
+        <c:axId val="160927920"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1014200208"/>
+        <c:axId val="160936624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="65"/>
@@ -2680,8 +2720,8 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Jumlah komponen</a:t>
+                  <a:rPr lang="en-US" i="1"/>
+                  <a:t>principal component</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -2753,13 +2793,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1014200752"/>
+        <c:crossAx val="160927920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1014200752"/>
+        <c:axId val="160927920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2872,7 +2912,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1014200208"/>
+        <c:crossAx val="160936624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2999,7 +3039,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3241,11 +3280,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-36"/>
-        <c:axId val="1014207824"/>
-        <c:axId val="1014210544"/>
+        <c:axId val="160924112"/>
+        <c:axId val="160925744"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1014207824"/>
+        <c:axId val="160924112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3282,7 +3321,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3349,7 +3387,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1014210544"/>
+        <c:crossAx val="160925744"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3357,7 +3395,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1014210544"/>
+        <c:axId val="160925744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3403,7 +3441,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3464,7 +3501,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1014207824"/>
+        <c:crossAx val="160924112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3478,7 +3515,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3896,11 +3932,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-36"/>
-        <c:axId val="1014210000"/>
-        <c:axId val="1014201840"/>
+        <c:axId val="160928464"/>
+        <c:axId val="47663712"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1014210000"/>
+        <c:axId val="160928464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4004,7 +4040,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1014201840"/>
+        <c:crossAx val="47663712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4012,7 +4048,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1014201840"/>
+        <c:axId val="47663712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4119,7 +4155,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1014210000"/>
+        <c:crossAx val="160928464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6953,16 +6989,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>171</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1082040</xdr:colOff>
+      <xdr:row>180</xdr:row>
+      <xdr:rowOff>34290</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>251460</xdr:colOff>
-      <xdr:row>194</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>594360</xdr:colOff>
+      <xdr:row>202</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7024,15 +7060,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>171</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>181</xdr:row>
+      <xdr:rowOff>110490</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>251460</xdr:colOff>
-      <xdr:row>194</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
+      <xdr:colOff>594360</xdr:colOff>
+      <xdr:row>205</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7391,10 +7427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:Z169"/>
+  <dimension ref="C3:Z174"/>
   <sheetViews>
-    <sheetView topLeftCell="G173" workbookViewId="0">
-      <selection activeCell="E57" sqref="E57"/>
+    <sheetView tabSelected="1" topLeftCell="A158" workbookViewId="0">
+      <selection activeCell="G172" sqref="G172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11027,10 +11063,10 @@
       </c>
     </row>
     <row r="55" spans="3:26" x14ac:dyDescent="0.3">
-      <c r="E55" s="12" t="s">
+      <c r="E55" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="F55" s="12"/>
+      <c r="F55" s="16"/>
       <c r="G55" s="7"/>
       <c r="H55" s="7"/>
     </row>
@@ -18236,34 +18272,35 @@
       </c>
     </row>
     <row r="166" spans="3:26" x14ac:dyDescent="0.3">
-      <c r="G166">
+      <c r="F166" s="12"/>
+      <c r="G166" s="12">
         <v>10</v>
       </c>
-      <c r="H166">
+      <c r="H166" s="12">
         <v>20</v>
       </c>
-      <c r="I166">
+      <c r="I166" s="12">
         <v>30</v>
       </c>
-      <c r="J166">
+      <c r="J166" s="12">
         <v>40</v>
       </c>
-      <c r="K166">
+      <c r="K166" s="12">
         <v>50</v>
       </c>
-      <c r="L166">
+      <c r="L166" s="12">
         <v>60</v>
       </c>
-      <c r="M166">
+      <c r="M166" s="12">
         <v>70</v>
       </c>
-      <c r="N166">
+      <c r="N166" s="12">
         <v>80</v>
       </c>
-      <c r="O166">
+      <c r="O166" s="12">
         <v>90</v>
       </c>
-      <c r="P166">
+      <c r="P166" s="12">
         <v>100</v>
       </c>
       <c r="Q166">
@@ -18298,37 +18335,37 @@
       </c>
     </row>
     <row r="167" spans="3:26" x14ac:dyDescent="0.3">
-      <c r="F167" t="s">
-        <v>1</v>
-      </c>
-      <c r="G167" s="5">
+      <c r="F167" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="G167" s="15">
         <v>0.77767999999999959</v>
       </c>
-      <c r="H167" s="5">
+      <c r="H167" s="15">
         <v>0.67100599999999988</v>
       </c>
-      <c r="I167" s="5">
+      <c r="I167" s="15">
         <v>0.64631000000000005</v>
       </c>
-      <c r="J167" s="5">
+      <c r="J167" s="15">
         <v>0.65527000000000013</v>
       </c>
-      <c r="K167" s="5">
+      <c r="K167" s="19">
         <v>0.86656800000000023</v>
       </c>
-      <c r="L167" s="5">
+      <c r="L167" s="19">
         <v>0.87021800000000016</v>
       </c>
-      <c r="M167" s="5">
+      <c r="M167" s="15">
         <v>0.87021800000000016</v>
       </c>
-      <c r="N167" s="5">
+      <c r="N167" s="15">
         <v>0.87021800000000016</v>
       </c>
-      <c r="O167" s="5">
+      <c r="O167" s="15">
         <v>0.87021800000000016</v>
       </c>
-      <c r="P167" s="5">
+      <c r="P167" s="15">
         <v>0.87021800000000016</v>
       </c>
       <c r="Q167" s="5">
@@ -18363,37 +18400,37 @@
       </c>
     </row>
     <row r="168" spans="3:26" x14ac:dyDescent="0.3">
-      <c r="F168" t="s">
+      <c r="F168" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G168" s="5">
+      <c r="G168" s="15">
         <v>0.74391999999999991</v>
       </c>
-      <c r="H168" s="5">
+      <c r="H168" s="15">
         <v>0.86453800000000003</v>
       </c>
-      <c r="I168" s="5">
+      <c r="I168" s="15">
         <v>0.93901000000000023</v>
       </c>
-      <c r="J168" s="5">
+      <c r="J168" s="15">
         <v>0.92940800000000012</v>
       </c>
-      <c r="K168" s="5">
+      <c r="K168" s="19">
         <v>0.79445600000000016</v>
       </c>
-      <c r="L168" s="5">
+      <c r="L168" s="19">
         <v>0.79249800000000004</v>
       </c>
-      <c r="M168" s="5">
+      <c r="M168" s="15">
         <v>0.79249800000000004</v>
       </c>
-      <c r="N168" s="5">
+      <c r="N168" s="15">
         <v>0.79249800000000004</v>
       </c>
-      <c r="O168" s="5">
+      <c r="O168" s="15">
         <v>0.79249800000000004</v>
       </c>
-      <c r="P168" s="5">
+      <c r="P168" s="15">
         <v>0.79249800000000004</v>
       </c>
       <c r="Q168" s="5">
@@ -18428,37 +18465,37 @@
       </c>
     </row>
     <row r="169" spans="3:26" x14ac:dyDescent="0.3">
-      <c r="F169" t="s">
+      <c r="F169" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="G169" s="5">
+      <c r="G169" s="15">
         <v>0.86312799999999978</v>
       </c>
-      <c r="H169" s="5">
+      <c r="H169" s="15">
         <v>0.57516199999999995</v>
       </c>
-      <c r="I169" s="5">
+      <c r="I169" s="15">
         <v>0.5129260000000001</v>
       </c>
-      <c r="J169" s="5">
+      <c r="J169" s="15">
         <v>0.53023400000000009</v>
       </c>
-      <c r="K169" s="5">
+      <c r="K169" s="19">
         <v>0.98660999999999999</v>
       </c>
-      <c r="L169" s="5">
+      <c r="L169" s="19">
         <v>0.995</v>
       </c>
-      <c r="M169" s="5">
+      <c r="M169" s="15">
         <v>0.995</v>
       </c>
-      <c r="N169" s="5">
+      <c r="N169" s="15">
         <v>0.995</v>
       </c>
-      <c r="O169" s="5">
+      <c r="O169" s="15">
         <v>0.995</v>
       </c>
-      <c r="P169" s="5">
+      <c r="P169" s="15">
         <v>0.995</v>
       </c>
       <c r="Q169" s="5">
@@ -18489,6 +18526,157 @@
         <v>0.995</v>
       </c>
       <c r="Z169" s="5">
+        <v>0.995</v>
+      </c>
+    </row>
+    <row r="170" spans="3:26" x14ac:dyDescent="0.3">
+      <c r="F170" s="20"/>
+      <c r="G170" s="20"/>
+      <c r="H170" s="20"/>
+      <c r="I170" s="20"/>
+      <c r="J170" s="20"/>
+      <c r="K170" s="20"/>
+      <c r="L170" s="20"/>
+      <c r="M170" s="20"/>
+      <c r="N170" s="20"/>
+      <c r="O170" s="20"/>
+      <c r="P170" s="20"/>
+    </row>
+    <row r="171" spans="3:26" x14ac:dyDescent="0.3">
+      <c r="F171" s="12"/>
+      <c r="G171" s="12">
+        <v>110</v>
+      </c>
+      <c r="H171" s="12">
+        <v>120</v>
+      </c>
+      <c r="I171" s="12">
+        <v>130</v>
+      </c>
+      <c r="J171" s="12">
+        <v>140</v>
+      </c>
+      <c r="K171" s="12">
+        <v>150</v>
+      </c>
+      <c r="L171" s="12">
+        <v>160</v>
+      </c>
+      <c r="M171" s="12">
+        <v>170</v>
+      </c>
+      <c r="N171" s="12">
+        <v>180</v>
+      </c>
+      <c r="O171" s="12">
+        <v>190</v>
+      </c>
+      <c r="P171" s="12">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="172" spans="3:26" x14ac:dyDescent="0.3">
+      <c r="F172" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="G172" s="15">
+        <v>0.87021800000000016</v>
+      </c>
+      <c r="H172" s="15">
+        <v>0.87021800000000016</v>
+      </c>
+      <c r="I172" s="15">
+        <v>0.87021800000000016</v>
+      </c>
+      <c r="J172" s="15">
+        <v>0.87021800000000016</v>
+      </c>
+      <c r="K172" s="15">
+        <v>0.87021800000000016</v>
+      </c>
+      <c r="L172" s="15">
+        <v>0.87021800000000016</v>
+      </c>
+      <c r="M172" s="15">
+        <v>0.87021800000000016</v>
+      </c>
+      <c r="N172" s="15">
+        <v>0.87021800000000016</v>
+      </c>
+      <c r="O172" s="15">
+        <v>0.87021800000000016</v>
+      </c>
+      <c r="P172" s="15">
+        <v>0.87021800000000016</v>
+      </c>
+    </row>
+    <row r="173" spans="3:26" x14ac:dyDescent="0.3">
+      <c r="F173" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="G173" s="15">
+        <v>0.79249800000000004</v>
+      </c>
+      <c r="H173" s="15">
+        <v>0.79249800000000004</v>
+      </c>
+      <c r="I173" s="15">
+        <v>0.79249800000000004</v>
+      </c>
+      <c r="J173" s="15">
+        <v>0.79249800000000004</v>
+      </c>
+      <c r="K173" s="15">
+        <v>0.79249800000000004</v>
+      </c>
+      <c r="L173" s="15">
+        <v>0.79249800000000004</v>
+      </c>
+      <c r="M173" s="15">
+        <v>0.79249800000000004</v>
+      </c>
+      <c r="N173" s="15">
+        <v>0.79249800000000004</v>
+      </c>
+      <c r="O173" s="15">
+        <v>0.79249800000000004</v>
+      </c>
+      <c r="P173" s="15">
+        <v>0.79249800000000004</v>
+      </c>
+    </row>
+    <row r="174" spans="3:26" x14ac:dyDescent="0.3">
+      <c r="F174" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="G174" s="15">
+        <v>0.995</v>
+      </c>
+      <c r="H174" s="15">
+        <v>0.995</v>
+      </c>
+      <c r="I174" s="15">
+        <v>0.995</v>
+      </c>
+      <c r="J174" s="15">
+        <v>0.995</v>
+      </c>
+      <c r="K174" s="15">
+        <v>0.995</v>
+      </c>
+      <c r="L174" s="15">
+        <v>0.995</v>
+      </c>
+      <c r="M174" s="15">
+        <v>0.995</v>
+      </c>
+      <c r="N174" s="15">
+        <v>0.995</v>
+      </c>
+      <c r="O174" s="15">
+        <v>0.995</v>
+      </c>
+      <c r="P174" s="15">
         <v>0.995</v>
       </c>
     </row>
@@ -19285,24 +19473,24 @@
       </c>
     </row>
     <row r="17" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C17" s="14" t="s">
+      <c r="C17" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="D17" s="13" t="s">
+      <c r="D17" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="13"/>
-      <c r="K17" s="13"/>
-      <c r="L17" s="13"/>
-      <c r="M17" s="13"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="17"/>
+      <c r="K17" s="17"/>
+      <c r="L17" s="17"/>
+      <c r="M17" s="17"/>
     </row>
     <row r="18" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C18" s="14"/>
+      <c r="C18" s="18"/>
       <c r="D18">
         <v>1</v>
       </c>
@@ -19556,8 +19744,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:AA169"/>
   <sheetViews>
-    <sheetView topLeftCell="E163" workbookViewId="0">
-      <selection activeCell="O113" sqref="O113:O162"/>
+    <sheetView topLeftCell="E157" workbookViewId="0">
+      <selection activeCell="V189" sqref="V189"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -36694,7 +36882,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:Z171"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D163" workbookViewId="0">
+    <sheetView topLeftCell="D163" workbookViewId="0">
       <selection activeCell="L171" sqref="L171"/>
     </sheetView>
   </sheetViews>
@@ -43116,46 +43304,46 @@
       <c r="Z164" s="5"/>
     </row>
     <row r="166" spans="3:26" x14ac:dyDescent="0.3">
-      <c r="F166" s="15"/>
-      <c r="G166" s="16" t="s">
+      <c r="F166" s="12"/>
+      <c r="G166" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="H166" s="17" t="s">
+      <c r="H166" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="I166" s="16" t="s">
+      <c r="I166" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="J166" s="17" t="s">
+      <c r="J166" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="K166" s="16" t="s">
+      <c r="K166" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="L166" s="17" t="s">
+      <c r="L166" s="14" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="167" spans="3:26" x14ac:dyDescent="0.3">
-      <c r="F167" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="G167" s="18">
+      <c r="F167" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="G167" s="15">
         <v>0.84758600000000006</v>
       </c>
-      <c r="H167" s="18">
+      <c r="H167" s="15">
         <v>0.82895399999999997</v>
       </c>
-      <c r="I167" s="18">
+      <c r="I167" s="15">
         <v>0.38746999999999993</v>
       </c>
-      <c r="J167" s="18">
+      <c r="J167" s="15">
         <v>0.36881399999999998</v>
       </c>
-      <c r="K167" s="18">
+      <c r="K167" s="15">
         <v>0.28156999999999999</v>
       </c>
-      <c r="L167" s="18">
+      <c r="L167" s="15">
         <v>0.19341599999999995</v>
       </c>
       <c r="M167" s="5"/>
@@ -43173,25 +43361,25 @@
       <c r="Z167" s="5"/>
     </row>
     <row r="168" spans="3:26" x14ac:dyDescent="0.3">
-      <c r="F168" s="15" t="s">
+      <c r="F168" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G168" s="18">
+      <c r="G168" s="15">
         <v>0.76448399999999983</v>
       </c>
-      <c r="H168" s="18">
+      <c r="H168" s="15">
         <v>0.74027400000000032</v>
       </c>
-      <c r="I168" s="18">
+      <c r="I168" s="15">
         <v>0.49225000000000002</v>
       </c>
-      <c r="J168" s="18">
+      <c r="J168" s="15">
         <v>0.41716600000000009</v>
       </c>
-      <c r="K168" s="18">
+      <c r="K168" s="15">
         <v>0.23591400000000001</v>
       </c>
-      <c r="L168" s="18">
+      <c r="L168" s="15">
         <v>0.16008399999999998</v>
       </c>
       <c r="M168" s="5"/>
@@ -43209,25 +43397,25 @@
       <c r="Z168" s="5"/>
     </row>
     <row r="169" spans="3:26" x14ac:dyDescent="0.3">
-      <c r="F169" s="15" t="s">
+      <c r="F169" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="G169" s="18">
+      <c r="G169" s="15">
         <v>0.99</v>
       </c>
-      <c r="H169" s="18">
+      <c r="H169" s="15">
         <v>0.98499999999999999</v>
       </c>
-      <c r="I169" s="18">
+      <c r="I169" s="15">
         <v>0.38241799999999981</v>
       </c>
-      <c r="J169" s="18">
+      <c r="J169" s="15">
         <v>0.40345000000000009</v>
       </c>
-      <c r="K169" s="18">
+      <c r="K169" s="15">
         <v>0.463752</v>
       </c>
-      <c r="L169" s="18">
+      <c r="L169" s="15">
         <v>0.316334</v>
       </c>
       <c r="M169" s="5"/>
@@ -43245,7 +43433,7 @@
       <c r="Z169" s="5"/>
     </row>
     <row r="171" spans="3:26" x14ac:dyDescent="0.3">
-      <c r="I171" s="15"/>
+      <c r="I171" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>